<commit_message>
Update employee management: add tour_number field to Employee model, implement validation for unique tour numbers, and adjust frontend components for tour number input and display. Change backend server port from 8000 to 9000.
</commit_message>
<xml_diff>
--- a/example_import_files/employee_examples.xlsx
+++ b/example_import_files/employee_examples.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markj/Documents/Studium/Master Maschinenbau TH Koeln/Digitalisierung/SAPV_route_optimization/example_import_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95DB41AC-8823-8740-B152-28070D5DBB48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D77678-F0F5-1649-B2B9-0C230A2D62C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2980" yWindow="2220" windowWidth="28240" windowHeight="17240" xr2:uid="{BE61D418-1F51-B847-91F0-443E93710B5C}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
     <t>Vorname</t>
   </si>
@@ -158,13 +158,16 @@
   </si>
   <si>
     <t>PDL</t>
+  </si>
+  <si>
+    <t>Tournummer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -307,6 +310,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -489,7 +498,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -619,6 +628,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -664,12 +684,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1047,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1974F7D-A888-AC42-A06C-0E9D8A2E0FFE}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1058,7 +1081,7 @@
     <col min="1" max="7" width="12.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1080,8 +1103,11 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1103,8 +1129,11 @@
       <c r="G2">
         <v>60</v>
       </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1126,8 +1155,11 @@
       <c r="G3">
         <v>100</v>
       </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1149,8 +1181,11 @@
       <c r="G4">
         <v>75</v>
       </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1172,8 +1207,11 @@
       <c r="G5">
         <v>100</v>
       </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1195,8 +1233,11 @@
       <c r="G6">
         <v>100</v>
       </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1218,8 +1259,11 @@
       <c r="G7">
         <v>100</v>
       </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1241,8 +1285,11 @@
       <c r="G8">
         <v>75</v>
       </c>
+      <c r="H8">
+        <v>7</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1264,8 +1311,11 @@
       <c r="G9">
         <v>50</v>
       </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1287,8 +1337,11 @@
       <c r="G10">
         <v>100</v>
       </c>
+      <c r="H10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1310,8 +1363,12 @@
       <c r="G11">
         <v>50</v>
       </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
 </worksheet>
 </file>
</xml_diff>